<commit_message>
add example values to proteomics, imaging and metabolomics templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/Imaging_assay.xlsx
+++ b/templates/dataplant/Imaging_assay.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="100">
   <si>
     <t>TEMPLATE</t>
   </si>
@@ -263,13 +263,19 @@
     <t>Term Accession Number (DPBO:1000120)</t>
   </si>
   <si>
-    <t>Output [Raw Data File]</t>
+    <t>Output [Data]</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>organelles</t>
+    <t>organelle</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>https://bioregistry.io/GO:0043226</t>
   </si>
   <si>
     <t xml:space="preserve">OperaLX spinning-disk confocal microscope (Perkin Elmer) </t>
@@ -290,31 +296,22 @@
     <t>DIC</t>
   </si>
   <si>
-    <t>MetaXpress software</t>
+    <t>DPBO</t>
+  </si>
+  <si>
+    <t>http://purl.org/nfdi4plants/ontology/dpbo/DPBO_1000191</t>
+  </si>
+  <si>
+    <t>MetaXpress Software</t>
+  </si>
+  <si>
+    <t>V6.1</t>
   </si>
   <si>
     <t>Image Dimension (XYZCT): 1376 x 1040 x 16 x 2 x 1</t>
   </si>
   <si>
     <t>OME-TIFF</t>
-  </si>
-  <si>
-    <t>single cells</t>
-  </si>
-  <si>
-    <t>epifluorescence microscope (IX-81; Olympus-Europe, Hamburg, Germany)</t>
-  </si>
-  <si>
-    <t>Cascade II 512 _ 512, Photometrics</t>
-  </si>
-  <si>
-    <t>FITC</t>
-  </si>
-  <si>
-    <t>TIFF</t>
-  </si>
-  <si>
-    <t>colony</t>
   </si>
 </sst>
 </file>
@@ -370,8 +367,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:AR4" totalsRowShown="1" headerRowCount="1">
-  <autoFilter ref="A1:AR4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" name="annotationTable" displayName="annotationTable" ref="A1:AR2" totalsRowShown="1" headerRowCount="1">
+  <autoFilter ref="A1:AR2">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -461,7 +458,7 @@
     <tableColumn id="41" name="Parameter [image file path]" totalsRowFunction="none"/>
     <tableColumn id="42" name="Term Source REF (DPBO:1000120)" totalsRowFunction="none"/>
     <tableColumn id="43" name="Term Accession Number (DPBO:1000120)" totalsRowFunction="none"/>
-    <tableColumn id="44" name="Output [Raw Data File]" totalsRowFunction="none"/>
+    <tableColumn id="44" name="Output [Data]" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -949,7 +946,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR4"/>
+  <dimension ref="A1:AR2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:44" x14ac:dyDescent="0.25">
@@ -1094,31 +1091,31 @@
         <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G2" t="s">
         <v>84</v>
       </c>
       <c r="H2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="I2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J2" t="s">
         <v>84</v>
       </c>
       <c r="K2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="L2" t="s">
         <v>84</v>
@@ -1127,7 +1124,7 @@
         <v>84</v>
       </c>
       <c r="N2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="O2" t="s">
         <v>84</v>
@@ -1136,16 +1133,16 @@
         <v>84</v>
       </c>
       <c r="Q2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="R2" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="S2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="T2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="U2" t="s">
         <v>84</v>
@@ -1163,7 +1160,7 @@
         <v>84</v>
       </c>
       <c r="Z2" t="s">
-        <v>84</v>
+        <v>97</v>
       </c>
       <c r="AA2" t="s">
         <v>84</v>
@@ -1190,7 +1187,7 @@
         <v>84</v>
       </c>
       <c r="AI2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="AJ2" t="s">
         <v>84</v>
@@ -1199,7 +1196,7 @@
         <v>84</v>
       </c>
       <c r="AL2" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="AM2" t="s">
         <v>84</v>
@@ -1217,274 +1214,6 @@
         <v>84</v>
       </c>
       <c r="AR2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H3" t="s">
-        <v>97</v>
-      </c>
-      <c r="I3" t="s">
-        <v>87</v>
-      </c>
-      <c r="J3" t="s">
-        <v>84</v>
-      </c>
-      <c r="K3" t="s">
-        <v>84</v>
-      </c>
-      <c r="L3" t="s">
-        <v>84</v>
-      </c>
-      <c r="M3" t="s">
-        <v>84</v>
-      </c>
-      <c r="N3" t="s">
-        <v>84</v>
-      </c>
-      <c r="O3" t="s">
-        <v>84</v>
-      </c>
-      <c r="P3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>98</v>
-      </c>
-      <c r="R3" t="s">
-        <v>84</v>
-      </c>
-      <c r="S3" t="s">
-        <v>84</v>
-      </c>
-      <c r="T3" t="s">
-        <v>84</v>
-      </c>
-      <c r="U3" t="s">
-        <v>84</v>
-      </c>
-      <c r="V3" t="s">
-        <v>84</v>
-      </c>
-      <c r="W3" t="s">
-        <v>84</v>
-      </c>
-      <c r="X3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL3" t="s">
-        <v>99</v>
-      </c>
-      <c r="AM3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AN3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B4" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" t="s">
-        <v>84</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" t="s">
-        <v>84</v>
-      </c>
-      <c r="H4" t="s">
-        <v>84</v>
-      </c>
-      <c r="I4" t="s">
-        <v>84</v>
-      </c>
-      <c r="J4" t="s">
-        <v>84</v>
-      </c>
-      <c r="K4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L4" t="s">
-        <v>84</v>
-      </c>
-      <c r="M4" t="s">
-        <v>84</v>
-      </c>
-      <c r="N4" t="s">
-        <v>84</v>
-      </c>
-      <c r="O4" t="s">
-        <v>84</v>
-      </c>
-      <c r="P4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" t="s">
-        <v>84</v>
-      </c>
-      <c r="S4" t="s">
-        <v>84</v>
-      </c>
-      <c r="T4" t="s">
-        <v>84</v>
-      </c>
-      <c r="U4" t="s">
-        <v>84</v>
-      </c>
-      <c r="V4" t="s">
-        <v>84</v>
-      </c>
-      <c r="W4" t="s">
-        <v>84</v>
-      </c>
-      <c r="X4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>84</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AK4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AL4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AO4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AP4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ4" t="s">
-        <v>84</v>
-      </c>
-      <c r="AR4" t="s">
         <v>84</v>
       </c>
     </row>

</xml_diff>